<commit_message>
pq add education_level and fixed small bugs
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\experiment_final\experiment_implementation\data\participant_questionnaire_toy_x_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cui/Documents/uzh/PhD/Projects/MeRID/repository/MeRID-eye-tracking/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E71E02-6BF4-4DEB-B5EB-4A394D5510F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3D9FA1-E826-1445-8739-452FBAAF97B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_questionnaire_questi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>pq_question_no</t>
   </si>
@@ -367,17 +367,53 @@
     <t>&gt;20 years</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you read in any other language(s) than </t>
-  </si>
-  <si>
     <t xml:space="preserve">In a typical week, how much time do you spend reading each type of material listed below: </t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>Please report the highest level of education you have completed</t>
+  </si>
+  <si>
+    <t>Less than primary education</t>
+  </si>
+  <si>
+    <t>Primary education</t>
+  </si>
+  <si>
+    <t>Lower secondary education</t>
+  </si>
+  <si>
+    <t>Upper secondary education</t>
+  </si>
+  <si>
+    <t>Post-secondary non-tertiary education</t>
+  </si>
+  <si>
+    <t>Short-cycle tertiary education</t>
+  </si>
+  <si>
+    <t>Bachelor&amp;apos;s or equivalent</t>
+  </si>
+  <si>
+    <t>Master&amp;apos;s or equivalent</t>
+  </si>
+  <si>
+    <t>Doctoral or equivalent</t>
+  </si>
+  <si>
+    <t>level_education</t>
+  </si>
+  <si>
+    <t>Do you read in any other language(s) than [insert current language]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +547,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -854,8 +902,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1231,18 +1281,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="74.296875" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1318,7 +1368,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1344,113 +1394,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
         <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>41</v>
       </c>
       <c r="O6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
@@ -1459,18 +1534,18 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>113</v>
@@ -1479,18 +1554,18 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>113</v>
@@ -1499,84 +1574,72 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
         <v>52</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" t="s">
         <v>53</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
@@ -1597,18 +1660,18 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>57</v>
@@ -1629,18 +1692,18 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>57</v>
@@ -1661,18 +1724,18 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
@@ -1693,18 +1756,18 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
         <v>57</v>
@@ -1725,18 +1788,18 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -1757,18 +1820,18 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -1789,137 +1852,140 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>83</v>
+      </c>
+      <c r="O21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>115</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="B22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L22" t="s">
         <v>84</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>88</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>89</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
         <v>90</v>
-      </c>
-      <c r="O22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" t="s">
-        <v>99</v>
-      </c>
-      <c r="K23" t="s">
-        <v>100</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>101</v>
       </c>
       <c r="O23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
-      </c>
-      <c r="L24" t="s">
-        <v>105</v>
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" t="s">
+        <v>100</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="O24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
         <v>103</v>
@@ -1934,23 +2000,52 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>109</v>
+      </c>
+      <c r="O26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>110</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>111</v>
       </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>